<commit_message>
started transfering previewd data to excel file (generate_analysis in Excel.py)
</commit_message>
<xml_diff>
--- a/Run1_all_data.xlsx
+++ b/Run1_all_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Vial #</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Load time (min)</t>
+  </si>
+  <si>
+    <t>Run(e) 1</t>
   </si>
 </sst>
 </file>
@@ -212,10 +215,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -531,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,892 +554,897 @@
     <col min="11" max="12" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="3">
-        <v>35714.845000000001</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>11</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="3">
+        <v>35714.845000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="3">
         <v>8679.2999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="3">
+      <c r="B4" s="7"/>
+      <c r="C4" s="3">
         <v>4746.2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="3">
         <v>0.60270000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="3">
-        <v>1.0084176343828599</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="3">
+        <v>1.0084176343828599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="3">
+      <c r="B7" s="7"/>
+      <c r="C7" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>81453</v>
-      </c>
-      <c r="D8">
-        <v>82138.641573386805</v>
-      </c>
-      <c r="E8">
-        <v>136284.45590407599</v>
-      </c>
-      <c r="F8">
-        <v>5.1344463246530703</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2">
-        <v>3.0503535047980401</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>20369.099999999999</v>
+        <v>81453</v>
       </c>
       <c r="D9">
-        <v>20540.559636507802</v>
+        <v>82138.641573386805</v>
       </c>
       <c r="E9">
-        <v>34080.902001838098</v>
+        <v>136284.45590407599</v>
       </c>
       <c r="F9">
-        <v>4.5325110804971596</v>
+        <v>5.1344463246530703</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2">
-        <v>2.4072578165336398</v>
+        <v>3.0503535047980401</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="5">
-        <v>5511</v>
+        <v>20369.099999999999</v>
       </c>
       <c r="D10">
-        <v>5557.3895830839201</v>
+        <v>20540.559636507802</v>
       </c>
       <c r="E10">
-        <v>9220.8222715844004</v>
+        <v>34080.902001838098</v>
       </c>
       <c r="F10">
-        <v>3.9647696512150801</v>
+        <v>4.5325110804971596</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2">
+        <v>2.4072578165336398</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5">
-        <v>2790.7</v>
+        <v>5511</v>
       </c>
       <c r="D11">
-        <v>2814.19109227224</v>
+        <v>5557.3895830839201</v>
       </c>
       <c r="E11">
-        <v>4669.3066073871496</v>
+        <v>9220.8222715844004</v>
       </c>
       <c r="F11">
-        <v>3.6692523925695699</v>
+        <v>3.9647696512150801</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="5">
-        <v>1933.8</v>
+        <v>2790.7</v>
       </c>
       <c r="D12">
-        <v>1950.07802136957</v>
+        <v>2814.19109227224</v>
       </c>
       <c r="E12">
-        <v>3235.5699707475801</v>
+        <v>4669.3066073871496</v>
       </c>
       <c r="F12">
-        <v>3.5099507960855898</v>
+        <v>3.6692523925695699</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="5">
-        <v>1456.8</v>
+        <v>1933.8</v>
       </c>
       <c r="D13">
-        <v>1469.06280976894</v>
+        <v>1950.07802136957</v>
       </c>
       <c r="E13">
-        <v>2437.4694039637402</v>
+        <v>3235.5699707475801</v>
       </c>
       <c r="F13">
-        <v>3.3869391729764802</v>
+        <v>3.5099507960855898</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="5">
-        <v>1159.5</v>
+        <v>1456.8</v>
       </c>
       <c r="D14">
-        <v>1169.2602470669201</v>
+        <v>1469.06280976894</v>
       </c>
       <c r="E14">
-        <v>1940.03691233934</v>
+        <v>2437.4694039637402</v>
       </c>
       <c r="F14">
-        <v>3.28780999316362</v>
+        <v>3.3869391729764802</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="5">
-        <v>1015.1</v>
+        <v>1159.5</v>
       </c>
       <c r="D15">
-        <v>1023.64474066204</v>
+        <v>1169.2602470669201</v>
       </c>
       <c r="E15">
-        <v>1698.4316254555099</v>
+        <v>1940.03691233934</v>
       </c>
       <c r="F15">
-        <v>3.2300480679649</v>
-      </c>
-      <c r="G15">
-        <v>0.86459094275784398</v>
-      </c>
-      <c r="I15">
-        <v>-1.83490635307762E-2</v>
-      </c>
-      <c r="J15">
-        <v>3.1836339010769299</v>
+        <v>3.28780999316362</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="5">
-        <v>882.4</v>
+        <v>1015.1</v>
       </c>
       <c r="D16">
-        <v>889.82772057943203</v>
+        <v>1023.64474066204</v>
       </c>
       <c r="E16">
-        <v>1476.4023902097799</v>
+        <v>1698.4316254555099</v>
       </c>
       <c r="F16">
-        <v>3.1692047396217502</v>
+        <v>3.2300480679649</v>
       </c>
       <c r="G16">
-        <v>0.87343690189051404</v>
+        <v>0.86459094275784398</v>
       </c>
       <c r="I16">
-        <v>-1.7074513936737701E-2</v>
+        <v>-1.83490635307762E-2</v>
       </c>
       <c r="J16">
-        <v>3.1423217977957099</v>
+        <v>3.1836339010769299</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="5">
-        <v>788.5</v>
+        <v>882.4</v>
       </c>
       <c r="D17">
-        <v>795.13730471088195</v>
+        <v>889.82772057943203</v>
       </c>
       <c r="E17">
-        <v>1319.29202706302</v>
+        <v>1476.4023902097799</v>
       </c>
       <c r="F17">
-        <v>3.1203409378545302</v>
+        <v>3.1692047396217502</v>
       </c>
       <c r="G17">
-        <v>0.88836861375086895</v>
+        <v>0.87343690189051404</v>
       </c>
       <c r="I17">
-        <v>-1.5755955992030501E-2</v>
+        <v>-1.7074513936737701E-2</v>
       </c>
       <c r="J17">
-        <v>3.0990333772382099</v>
+        <v>3.1423217977957099</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="5">
-        <v>11.5</v>
+        <v>10</v>
       </c>
       <c r="C18" s="5">
-        <v>801.7</v>
+        <v>788.5</v>
       </c>
       <c r="D18">
-        <v>808.44841748473596</v>
+        <v>795.13730471088195</v>
       </c>
       <c r="E18">
-        <v>894.25188594074996</v>
+        <v>1319.29202706302</v>
       </c>
       <c r="F18">
-        <v>2.9514598647313202</v>
+        <v>3.1203409378545302</v>
       </c>
       <c r="G18">
-        <v>0.92253404114800497</v>
+        <v>0.88836861375086895</v>
       </c>
       <c r="I18">
-        <v>-1.4291015294764399E-2</v>
+        <v>-1.5755955992030501E-2</v>
       </c>
       <c r="J18">
-        <v>3.0503535047980401</v>
+        <v>3.0990333772382099</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="5">
-        <v>13</v>
+        <v>11.5</v>
       </c>
       <c r="C19" s="5">
-        <v>698.5</v>
+        <v>801.7</v>
       </c>
       <c r="D19">
-        <v>704.37971761642495</v>
+        <v>808.44841748473596</v>
       </c>
       <c r="E19">
-        <v>779.13800964152904</v>
+        <v>894.25188594074996</v>
       </c>
       <c r="F19">
-        <v>2.8916143915841301</v>
+        <v>2.9514598647313202</v>
       </c>
       <c r="G19">
-        <v>0.91811616913777605</v>
+        <v>0.92253404114800497</v>
       </c>
       <c r="I19">
-        <v>-1.3704013610313001E-2</v>
+        <v>-1.4291015294764399E-2</v>
       </c>
       <c r="J19">
-        <v>3.0305034558366302</v>
+        <v>3.0503535047980401</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" s="5">
         <v>13</v>
       </c>
-      <c r="B20" s="5">
-        <v>14.5</v>
-      </c>
       <c r="C20" s="5">
-        <v>647.9</v>
+        <v>698.5</v>
       </c>
       <c r="D20">
-        <v>653.35378531665197</v>
+        <v>704.37971761642495</v>
       </c>
       <c r="E20">
-        <v>722.69651602970202</v>
+        <v>779.13800964152904</v>
       </c>
       <c r="F20">
-        <v>2.8589559610792601</v>
+        <v>2.8916143915841301</v>
       </c>
       <c r="G20">
-        <v>0.907602322472293</v>
+        <v>0.91811616913777605</v>
       </c>
       <c r="I20">
-        <v>-1.33163780682993E-2</v>
+        <v>-1.3704013610313001E-2</v>
       </c>
       <c r="J20">
-        <v>3.0171668823119302</v>
+        <v>3.0305034558366302</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="5">
-        <v>16</v>
+        <v>14.5</v>
       </c>
       <c r="C21" s="5">
-        <v>629.29999999999995</v>
+        <v>647.9</v>
       </c>
       <c r="D21">
-        <v>634.59721731713103</v>
+        <v>653.35378531665197</v>
       </c>
       <c r="E21">
-        <v>701.94924762693495</v>
+        <v>722.69651602970202</v>
       </c>
       <c r="F21">
-        <v>2.8463057128814202</v>
+        <v>2.8589559610792601</v>
       </c>
       <c r="G21">
-        <v>0.89420888924428499</v>
+        <v>0.907602322472293</v>
       </c>
       <c r="I21">
-        <v>-1.2934937716161001E-2</v>
+        <v>-1.33163780682993E-2</v>
       </c>
       <c r="J21">
-        <v>3.0038179541907901</v>
+        <v>3.0171668823119302</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="5">
-        <v>17.5</v>
+        <v>16</v>
       </c>
       <c r="C22" s="5">
-        <v>622.20000000000005</v>
+        <v>629.29999999999995</v>
       </c>
       <c r="D22">
-        <v>627.43745211301302</v>
+        <v>634.59721731713103</v>
       </c>
       <c r="E22">
-        <v>694.02959140867495</v>
+        <v>701.94924762693495</v>
       </c>
       <c r="F22">
-        <v>2.8413779879066201</v>
+        <v>2.8463057128814202</v>
       </c>
       <c r="G22">
-        <v>0.881055501539313</v>
+        <v>0.89420888924428499</v>
       </c>
       <c r="I22">
-        <v>-1.2331316310186901E-2</v>
+        <v>-1.2934937716161001E-2</v>
       </c>
       <c r="J22">
-        <v>2.9823359418431901</v>
+        <v>3.0038179541907901</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="5">
-        <v>19</v>
+        <v>17.5</v>
       </c>
       <c r="C23" s="5">
-        <v>507.9</v>
+        <v>622.20000000000005</v>
       </c>
       <c r="D23">
-        <v>512.17531650305295</v>
+        <v>627.43745211301302</v>
       </c>
       <c r="E23">
-        <v>566.53428074006104</v>
+        <v>694.02959140867495</v>
       </c>
       <c r="F23">
-        <v>2.7532261939625302</v>
+        <v>2.8413779879066201</v>
       </c>
       <c r="G23">
-        <v>0.88138214581505603</v>
+        <v>0.881055501539313</v>
       </c>
       <c r="I23">
-        <v>-1.1302032670781699E-2</v>
+        <v>-1.2331316310186901E-2</v>
       </c>
       <c r="J23">
-        <v>2.94509571570905</v>
+        <v>2.9823359418431901</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="5">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="C24" s="5">
-        <v>504.2</v>
+        <v>507.9</v>
       </c>
       <c r="D24">
-        <v>508.44417125583601</v>
+        <v>512.17531650305295</v>
       </c>
       <c r="E24">
-        <v>562.40713595026398</v>
+        <v>566.53428074006104</v>
       </c>
       <c r="F24">
-        <v>2.7500508224743601</v>
+        <v>2.7532261939625302</v>
       </c>
       <c r="G24">
-        <v>0.85860789728371001</v>
+        <v>0.88138214581505603</v>
       </c>
       <c r="I24">
-        <v>-1.09434917119095E-2</v>
+        <v>-1.1302032670781699E-2</v>
       </c>
       <c r="J24">
-        <v>2.9319120677483501</v>
+        <v>2.94509571570905</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="5">
-        <v>22</v>
+        <v>20.5</v>
       </c>
       <c r="C25" s="5">
-        <v>422.8</v>
+        <v>504.2</v>
       </c>
       <c r="D25">
-        <v>426.35897581707201</v>
+        <v>508.44417125583601</v>
       </c>
       <c r="E25">
-        <v>471.60995057471501</v>
+        <v>562.40713595026398</v>
       </c>
       <c r="F25">
-        <v>2.6735829597693201</v>
+        <v>2.7500508224743601</v>
       </c>
       <c r="G25">
-        <v>0.83448711305216605</v>
+        <v>0.85860789728371001</v>
       </c>
       <c r="I25">
-        <v>-1.01724896191135E-2</v>
+        <v>-1.09434917119095E-2</v>
       </c>
       <c r="J25">
-        <v>2.9031123188430601</v>
+        <v>2.9319120677483501</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="5">
-        <v>23.5</v>
+        <v>22</v>
       </c>
       <c r="C26" s="5">
-        <v>451.9</v>
+        <v>422.8</v>
       </c>
       <c r="D26">
-        <v>455.70392897761297</v>
+        <v>426.35897581707201</v>
       </c>
       <c r="E26">
-        <v>504.06938662420498</v>
+        <v>471.60995057471501</v>
       </c>
       <c r="F26">
-        <v>2.7024903224651302</v>
+        <v>2.6735829597693201</v>
       </c>
       <c r="G26">
-        <v>0.80705994728868302</v>
+        <v>0.83448711305216605</v>
       </c>
       <c r="I26">
-        <v>-1.02955302497225E-2</v>
+        <v>-1.01724896191135E-2</v>
       </c>
       <c r="J26">
-        <v>2.90777870926448</v>
+        <v>2.9031123188430601</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="5">
-        <v>25</v>
+        <v>23.5</v>
       </c>
       <c r="C27" s="5">
-        <v>411.3</v>
+        <v>451.9</v>
       </c>
       <c r="D27">
-        <v>414.76217302166901</v>
+        <v>455.70392897761297</v>
       </c>
       <c r="E27">
-        <v>458.78233839020902</v>
+        <v>504.06938662420498</v>
       </c>
       <c r="F27">
-        <v>2.6616066906431102</v>
+        <v>2.7024903224651302</v>
       </c>
       <c r="G27">
-        <v>0.75644105001412798</v>
+        <v>0.80705994728868302</v>
       </c>
       <c r="I27">
-        <v>-9.3374607001882794E-3</v>
+        <v>-1.02955302497225E-2</v>
       </c>
       <c r="J27">
-        <v>2.8709138592063201</v>
+        <v>2.90777870926448</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="5">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="5">
-        <v>475.7</v>
+        <v>411.3</v>
       </c>
       <c r="D28">
-        <v>479.70426867592499</v>
+        <v>414.76217302166901</v>
       </c>
       <c r="E28">
-        <v>397.96272496758297</v>
+        <v>458.78233839020902</v>
       </c>
       <c r="F28">
-        <v>2.5998423959455299</v>
+        <v>2.6616066906431102</v>
       </c>
       <c r="G28">
-        <v>0.67635488015826695</v>
+        <v>0.75644105001412798</v>
       </c>
       <c r="I28">
-        <v>-8.5331490688050297E-3</v>
+        <v>-9.3374607001882794E-3</v>
       </c>
       <c r="J28">
-        <v>2.8395457055823701</v>
+        <v>2.8709138592063201</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" s="5">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
-        <v>453.3</v>
+        <v>475.7</v>
       </c>
       <c r="D29">
-        <v>457.11571366574901</v>
+        <v>479.70426867592499</v>
       </c>
       <c r="E29">
-        <v>379.22325673282597</v>
+        <v>397.96272496758297</v>
       </c>
       <c r="F29">
-        <v>2.5788949635843199</v>
+        <v>2.5998423959455299</v>
       </c>
       <c r="G29">
-        <v>0.62693584246562595</v>
+        <v>0.67635488015826695</v>
       </c>
       <c r="I29">
-        <v>-8.9209942679341694E-3</v>
+        <v>-8.5331490688050297E-3</v>
       </c>
       <c r="J29">
-        <v>2.8549302318144898</v>
+        <v>2.8395457055823701</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="5">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="5">
-        <v>467.4</v>
+        <v>453.3</v>
       </c>
       <c r="D30">
-        <v>471.33440231054698</v>
+        <v>457.11571366574901</v>
       </c>
       <c r="E30">
-        <v>391.01908271988299</v>
+        <v>379.22325673282597</v>
       </c>
       <c r="F30">
-        <v>2.5921979525818402</v>
+        <v>2.5788949635843199</v>
       </c>
       <c r="G30">
-        <v>0.59959088656044701</v>
+        <v>0.62693584246562595</v>
       </c>
       <c r="I30">
-        <v>-9.8491961140098408E-3</v>
+        <v>-8.9209942679341694E-3</v>
       </c>
       <c r="J30">
-        <v>2.8923677062728799</v>
+        <v>2.8549302318144898</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="5">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="5">
-        <v>431.2</v>
+        <v>467.4</v>
       </c>
       <c r="D31">
-        <v>434.82968394588801</v>
+        <v>471.33440231054698</v>
       </c>
       <c r="E31">
-        <v>360.73476351906999</v>
+        <v>391.01908271988299</v>
       </c>
       <c r="F31">
-        <v>2.5571879967043101</v>
+        <v>2.5921979525818402</v>
       </c>
       <c r="G31">
-        <v>0.48157883151368902</v>
+        <v>0.59959088656044701</v>
       </c>
       <c r="I31">
-        <v>-9.4809585537764599E-3</v>
+        <v>-9.8491961140098408E-3</v>
       </c>
       <c r="J31">
-        <v>2.8772699663033099</v>
+        <v>2.8923677062728799</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="5">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C32" s="5">
-        <v>404.4</v>
+        <v>431.2</v>
       </c>
       <c r="D32">
-        <v>407.80409134442698</v>
+        <v>434.82968394588801</v>
       </c>
       <c r="E32">
-        <v>338.31432830962899</v>
+        <v>360.73476351906999</v>
       </c>
       <c r="F32">
-        <v>2.5293203914446001</v>
+        <v>2.5571879967043101</v>
       </c>
       <c r="G32">
-        <v>0.404167145119459</v>
+        <v>0.48157883151368902</v>
       </c>
       <c r="I32">
-        <v>-1.0201992286213501E-2</v>
+        <v>-9.4809585537764599E-3</v>
       </c>
       <c r="J32">
-        <v>2.90731303848818</v>
+        <v>2.8772699663033099</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="5">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C33" s="5">
-        <v>432.2</v>
+        <v>404.4</v>
       </c>
       <c r="D33">
-        <v>435.83810158027001</v>
+        <v>407.80409134442698</v>
       </c>
       <c r="E33">
-        <v>361.571346922408</v>
+        <v>338.31432830962899</v>
       </c>
       <c r="F33">
-        <v>2.5581940070728502</v>
+        <v>2.5293203914446001</v>
       </c>
       <c r="G33">
-        <v>0.42022818382638599</v>
+        <v>0.404167145119459</v>
       </c>
       <c r="I33">
-        <v>-1.3340429840131099E-2</v>
+        <v>-1.0201992286213501E-2</v>
       </c>
       <c r="J33">
-        <v>3.0401735616040302</v>
+        <v>2.90731303848818</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="5">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5">
-        <v>363.8</v>
+        <v>432.2</v>
       </c>
       <c r="D34">
-        <v>366.86233538848302</v>
+        <v>435.83810158027001</v>
       </c>
       <c r="E34">
-        <v>304.34904213413199</v>
+        <v>361.571346922408</v>
       </c>
       <c r="F34">
-        <v>2.4833719392531002</v>
+        <v>2.5581940070728502</v>
       </c>
       <c r="G34">
-        <v>0.18678431533977599</v>
+        <v>0.42022818382638599</v>
       </c>
       <c r="I34">
-        <v>-1.04363424517121E-2</v>
+        <v>-1.3340429840131099E-2</v>
       </c>
       <c r="J34">
-        <v>2.9152978039020101</v>
+        <v>3.0401735616040302</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="5">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C35" s="5">
-        <v>429.8</v>
+        <v>363.8</v>
       </c>
       <c r="D35">
-        <v>433.41789925775203</v>
+        <v>366.86233538848302</v>
       </c>
       <c r="E35">
-        <v>359.56354675439798</v>
+        <v>304.34904213413199</v>
       </c>
       <c r="F35">
-        <v>2.5557756556810598</v>
+        <v>2.4833719392531002</v>
+      </c>
+      <c r="G35">
+        <v>0.18678431533977599</v>
+      </c>
+      <c r="I35">
+        <v>-1.04363424517121E-2</v>
+      </c>
+      <c r="J35">
+        <v>2.9152978039020101</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="5">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C36" s="5">
-        <v>303.39999999999998</v>
+        <v>429.8</v>
       </c>
       <c r="D36">
-        <v>305.95391027175901</v>
+        <v>433.41789925775203</v>
       </c>
       <c r="E36">
-        <v>253.81940457255499</v>
+        <v>359.56354675439798</v>
       </c>
       <c r="F36">
-        <v>2.4045248209763401</v>
+        <v>2.5557756556810598</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
+        <v>29</v>
+      </c>
+      <c r="B37" s="5">
+        <v>43</v>
+      </c>
+      <c r="C37" s="5">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="D37">
+        <v>305.95391027175901</v>
+      </c>
+      <c r="E37">
+        <v>253.81940457255499</v>
+      </c>
+      <c r="F37">
+        <v>2.4045248209763401</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>30</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B38" s="6">
         <v>45</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C38" s="6">
         <v>348.1</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <v>351.03017852867202</v>
       </c>
-      <c r="E37">
+      <c r="E38">
         <v>291.21468270173602</v>
       </c>
-      <c r="F37">
+      <c r="F38">
         <v>2.46421326780992</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>